<commit_message>
Adding updated task list
</commit_message>
<xml_diff>
--- a/Task_List.xlsx
+++ b/Task_List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedef\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\CISS346\CISS346-Assignment5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC6830A-A676-40AE-9386-18804CE43F2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCC2F34-CAE7-4968-A562-5DB3B4D4CEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A93A2899-7AB8-4092-8440-AEB4946A1195}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{A93A2899-7AB8-4092-8440-AEB4946A1195}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Priority 1 Tasks</t>
   </si>
@@ -66,17 +66,41 @@
   </si>
   <si>
     <t>Server only displays all messages no matter priority that is selected to display, Add priority filtering</t>
+  </si>
+  <si>
+    <t>Server crashes when 'Messages.txt' doesn’t exist and the show messages button is pressed</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Producer crashes when server is offline, need message box to display no message available</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Server does not notify user when there are no messages to display</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Conumer crashes when requesting a message priority that isnt in the file</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumer crashes when server is offline, does not notify user</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -84,7 +108,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -92,6 +116,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -487,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECE80A5-9A34-4DE4-B150-19EF045529B6}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="151.33203125" customWidth="1"/>
   </cols>
@@ -503,8 +534,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:6" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -524,7 +555,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -566,7 +597,105 @@
         <v>Yes</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>20</v>
+      </c>
+      <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>